<commit_message>
Switching search terms to xlsx
</commit_message>
<xml_diff>
--- a/metadata/transformation_parameters_template.xlsx
+++ b/metadata/transformation_parameters_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danhopp/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/externalssd/dhopp1/nlp_pipeline_frontend/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96D655A2-17DA-3744-BBC3-90A84E6CA0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1EAD24-6BDD-AB48-ADC5-57DC778D941B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="17240" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{78F1ED48-8B3A-F84F-AD64-BBC0BEF13862}"/>
+    <workbookView xWindow="7840" yWindow="17240" windowWidth="28040" windowHeight="17440" xr2:uid="{78F1ED48-8B3A-F84F-AD64-BBC0BEF13862}"/>
   </bookViews>
   <sheets>
     <sheet name="prepunctuation" sheetId="1" r:id="rId1"/>
@@ -432,9 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357E6B16-5055-C74E-ADFD-B02B7932B42A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -494,7 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C69C8E-DFD8-0345-ABAA-FAE7A1A5F6B9}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>